<commit_message>
modified:   main.py 	modified:   users_info.xlsx
</commit_message>
<xml_diff>
--- a/users_info.xlsx
+++ b/users_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zyf13\Desktop\Projects\auto_xiuxian\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808B3CDE-EC70-490F-A05B-8C3B9CC746C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0805795C-4EE0-4191-8FCB-464D094CE2CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="42">
   <si>
     <t>users</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>xiu_lian_buy_times</t>
+  </si>
+  <si>
+    <t>dao_chang_level</t>
   </si>
 </sst>
 </file>
@@ -171,7 +174,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -179,13 +182,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -468,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -492,457 +513,485 @@
     <col min="14" max="14" width="15.15234375" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20.3046875" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16.84375" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.23046875" style="1"/>
+    <col min="17" max="17" width="14.69140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.23046875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="Q1" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
         <v>13679283735</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2" s="2">
         <v>0</v>
       </c>
-      <c r="J2" s="1">
-        <v>2</v>
-      </c>
-      <c r="K2" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="L2" s="1" t="s">
+      <c r="J2" s="2">
+        <v>2</v>
+      </c>
+      <c r="K2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="1">
+      <c r="M2" s="2">
         <v>0</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="P2" s="1">
-        <v>1</v>
+      <c r="P2" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>17633025505</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="1">
-        <v>2</v>
-      </c>
-      <c r="J3" s="1">
-        <v>2</v>
-      </c>
-      <c r="K3" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="L3" s="1" t="s">
+      <c r="I3" s="2">
+        <v>2</v>
+      </c>
+      <c r="J3" s="2">
+        <v>2</v>
+      </c>
+      <c r="K3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="M3" s="1">
-        <v>2</v>
-      </c>
-      <c r="N3" s="1" t="s">
+      <c r="M3" s="2">
+        <v>2</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="O3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="P3" s="1">
-        <v>1</v>
+      <c r="P3" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>18034447843</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="1">
-        <v>2</v>
-      </c>
-      <c r="J4" s="1">
-        <v>2</v>
-      </c>
-      <c r="K4" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="L4" s="1" t="s">
+      <c r="I4" s="2">
+        <v>2</v>
+      </c>
+      <c r="J4" s="2">
+        <v>2</v>
+      </c>
+      <c r="K4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="1">
-        <v>2</v>
-      </c>
-      <c r="N4" s="1" t="s">
+      <c r="M4" s="2">
+        <v>2</v>
+      </c>
+      <c r="N4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="O4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="P4" s="1">
-        <v>1</v>
+      <c r="P4" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>18116516860</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="1">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="2">
         <v>0</v>
       </c>
-      <c r="J5" s="1">
-        <v>2</v>
-      </c>
-      <c r="K5" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="L5" s="1" t="s">
+      <c r="J5" s="2">
+        <v>2</v>
+      </c>
+      <c r="K5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="M5" s="1">
+      <c r="M5" s="2">
         <v>0</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="N5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="O5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="P5" s="1">
-        <v>1</v>
+      <c r="P5" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="1">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="1">
-        <v>2</v>
-      </c>
-      <c r="J6" s="1">
-        <v>2</v>
-      </c>
-      <c r="K6" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="L6" s="1" t="s">
+      <c r="I6" s="2">
+        <v>2</v>
+      </c>
+      <c r="J6" s="2">
+        <v>2</v>
+      </c>
+      <c r="K6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="M6" s="1">
-        <v>2</v>
-      </c>
-      <c r="N6" s="1" t="s">
+      <c r="M6" s="2">
+        <v>2</v>
+      </c>
+      <c r="N6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="O6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="P6" s="1">
-        <v>1</v>
+      <c r="P6" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A7" s="1">
         <v>15157717132</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="1">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1" t="s">
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="1">
-        <v>2</v>
-      </c>
-      <c r="J7" s="1">
-        <v>2</v>
-      </c>
-      <c r="K7" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="L7" s="1" t="s">
+      <c r="I7" s="2">
+        <v>2</v>
+      </c>
+      <c r="J7" s="2">
+        <v>2</v>
+      </c>
+      <c r="K7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="M7" s="1">
-        <v>2</v>
-      </c>
-      <c r="N7" s="1" t="s">
+      <c r="M7" s="2">
+        <v>2</v>
+      </c>
+      <c r="N7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="O7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="P7" s="1">
-        <v>1</v>
+      <c r="P7" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A8" s="1">
         <v>13681801870</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="2">
         <v>4</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I8" s="1">
-        <v>3</v>
-      </c>
-      <c r="J8" s="1">
-        <v>3</v>
-      </c>
-      <c r="K8" s="1" t="b">
+      <c r="I8" s="2">
+        <v>3</v>
+      </c>
+      <c r="J8" s="2">
+        <v>3</v>
+      </c>
+      <c r="K8" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="L8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="M8" s="1">
-        <v>3</v>
-      </c>
-      <c r="N8" s="1" t="s">
+      <c r="M8" s="2">
+        <v>3</v>
+      </c>
+      <c r="N8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="O8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P8" s="1">
-        <v>3</v>
+      <c r="P8" s="2">
+        <v>3</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A9" s="1">
         <v>18915964295</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="1">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1" t="s">
+      <c r="E9" s="2">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="1">
-        <v>2</v>
-      </c>
-      <c r="J9" s="1">
-        <v>2</v>
-      </c>
-      <c r="K9" s="1" t="b">
+      <c r="I9" s="2">
+        <v>2</v>
+      </c>
+      <c r="J9" s="2">
+        <v>2</v>
+      </c>
+      <c r="K9" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="L9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="M9" s="1">
-        <v>2</v>
-      </c>
-      <c r="N9" s="1" t="s">
+      <c r="M9" s="2">
+        <v>2</v>
+      </c>
+      <c r="N9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="O9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="P9" s="1">
-        <v>2</v>
+      <c r="P9" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>